<commit_message>
add tax data from many countries
</commit_message>
<xml_diff>
--- a/input_data/admin_data/DOM/IR-1 consolidado (2012-2020).xlsx
+++ b/input_data/admin_data/DOM/IR-1 consolidado (2012-2020).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omena\Dropbox\LATAM-WIL\Data\Tax-data\DOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\i.flores.PSE\Documents\GitHub\dina-latam\input_data\admin_data\DOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB943C9-76AB-4068-BB8E-116F320D3D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96461374-6B3C-44E9-8D9A-6848088D2F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6195" yWindow="15" windowWidth="18165" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Año 2020" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="52">
   <si>
     <t xml:space="preserve">Hombres </t>
   </si>
@@ -463,17 +462,14 @@
   <si>
     <t>16/ Corresponde a la sumatoria de alquileres, dividendos e intereses, ver notas 3, 4 y 5.</t>
   </si>
-  <si>
-    <t>u</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14">
@@ -802,7 +798,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
@@ -869,43 +865,43 @@
     <xf numFmtId="165" fontId="0" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -914,13 +910,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -954,7 +950,7 @@
     <xf numFmtId="10" fontId="0" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -962,12 +958,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1027,9 +1023,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1047,7 +1043,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2258,36 +2254,36 @@
   <dimension ref="A1:AB52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="18.8984375" style="11" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="11" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="13.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -2362,7 +2358,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -3352,8 +3348,8 @@
       <c r="F16" s="30">
         <v>17457013296.57</v>
       </c>
-      <c r="G16" s="29" t="s">
-        <v>52</v>
+      <c r="G16" s="29">
+        <v>3557684.54</v>
       </c>
       <c r="H16" s="29">
         <v>17146001.859999999</v>
@@ -5038,33 +5034,33 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="13.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -5139,7 +5135,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -7816,30 +7812,30 @@
       <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="13.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -7914,7 +7910,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -10679,30 +10675,30 @@
       <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="17.69921875" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="13.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="17.75" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -10777,7 +10773,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -13454,31 +13450,31 @@
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="14.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -13553,7 +13549,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -16230,31 +16226,31 @@
       <selection pane="bottomRight" activeCell="E23" sqref="E23:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="14.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -16329,7 +16325,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -19006,31 +19002,31 @@
       <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="14.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -19105,7 +19101,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -21782,31 +21778,31 @@
       <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="14.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -21881,7 +21877,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -24558,31 +24554,31 @@
       <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.69921875" customWidth="1"/>
-    <col min="15" max="16" width="20.59765625" customWidth="1"/>
-    <col min="17" max="19" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.59765625" style="18" customWidth="1"/>
-    <col min="22" max="22" width="19.69921875" style="11" customWidth="1"/>
-    <col min="23" max="23" width="22.3984375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="23.69921875" customWidth="1"/>
-    <col min="25" max="26" width="23.69921875" style="11" customWidth="1"/>
-    <col min="27" max="27" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" customWidth="1"/>
+    <col min="15" max="16" width="20.625" customWidth="1"/>
+    <col min="17" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.625" style="18" customWidth="1"/>
+    <col min="22" max="22" width="19.75" style="11" customWidth="1"/>
+    <col min="23" max="23" width="22.375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="23.75" customWidth="1"/>
+    <col min="25" max="26" width="23.75" style="11" customWidth="1"/>
+    <col min="27" max="27" width="14.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="54.9" customHeight="1">
+    <row r="1" spans="1:27" ht="54.95" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="68" t="s">
@@ -24657,7 +24653,7 @@
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="48.6">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="49.5">
       <c r="A3" s="67"/>
       <c r="B3" s="7" t="s">
         <v>3</v>

</xml_diff>